<commit_message>
Updated calibration summary scripts and outputs
Updated calibration summary scripts and outputs to reflect changes in the CVM Estimation and Calibration document related to summarizing Establishment and TNC Routes by time period.
</commit_message>
<xml_diff>
--- a/Calib_Summary/CVM_Calibration_Template.xlsx
+++ b/Calib_Summary/CVM_Calibration_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VY-Projects\SANDAG_CVM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgliebe\Documents\Projects\SANDAG\Final Summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E405CF2-896E-4C81-A7E5-18C9F00D37C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5260DA20-C117-4CB4-991A-4DB646E991A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="854" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28230" yWindow="-450" windowWidth="28155" windowHeight="13320" tabRatio="854" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Household Attractor" sheetId="6" r:id="rId1"/>
@@ -426,9 +426,6 @@
     <t>% Share</t>
   </si>
   <si>
-    <t>CVM Trips</t>
-  </si>
-  <si>
     <t>Time Period</t>
   </si>
   <si>
@@ -459,9 +456,6 @@
     <t>EA</t>
   </si>
   <si>
-    <t>TNC</t>
-  </si>
-  <si>
     <t>Origination Type</t>
   </si>
   <si>
@@ -634,6 +628,12 @@
   </si>
   <si>
     <t>TNC_Retail</t>
+  </si>
+  <si>
+    <t>CVM Routes</t>
+  </si>
+  <si>
+    <t>TNC Routes</t>
   </si>
 </sst>
 </file>
@@ -815,6 +815,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -878,6 +879,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="42">
@@ -3321,25 +3323,25 @@
       <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.52734375" customWidth="1"/>
-    <col min="2" max="2" width="1.76171875" customWidth="1"/>
+    <col min="1" max="1" width="8.54296875" customWidth="1"/>
+    <col min="2" max="2" width="1.7265625" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.234375" customWidth="1"/>
-    <col min="11" max="11" width="3.76171875" customWidth="1"/>
+    <col min="7" max="7" width="3.26953125" customWidth="1"/>
+    <col min="11" max="11" width="3.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C1" s="24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C2" s="24"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C4" s="60" t="s">
         <v>1</v>
       </c>
@@ -3353,7 +3355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C5" s="17" t="s">
         <v>5</v>
       </c>
@@ -3370,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C6" s="17" t="s">
         <v>6</v>
       </c>
@@ -3387,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C7" s="17" t="s">
         <v>7</v>
       </c>
@@ -3404,10 +3406,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F8" s="43"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C11" s="131" t="s">
         <v>8</v>
       </c>
@@ -3429,7 +3431,7 @@
       <c r="M11" s="130"/>
       <c r="N11" s="130"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C12" s="132"/>
       <c r="D12" s="17" t="s">
         <v>5</v>
@@ -3461,7 +3463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>0</v>
       </c>
@@ -3489,7 +3491,7 @@
       <c r="M13" s="23"/>
       <c r="N13" s="23"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B14" s="17">
         <v>1</v>
       </c>
@@ -3535,7 +3537,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B15" s="17">
         <v>2</v>
       </c>
@@ -3581,7 +3583,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B16" s="17">
         <v>3</v>
       </c>
@@ -3627,7 +3629,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B17" s="17">
         <v>4</v>
       </c>
@@ -3673,17 +3675,17 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C21" s="24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C22" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C23" s="24" t="s">
         <v>16</v>
       </c>
@@ -3707,26 +3709,26 @@
       <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="14.234375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.76171875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.76171875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.76171875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.234375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.41015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="14" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.87890625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.41015625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="14" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="20.52734375" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="9.234375" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="9.234375" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="20.76171875" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="11.1171875" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="13.234375" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="12.234375" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="18.52734375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3737,11 +3739,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6180C7-702D-4C2B-A1ED-2B991261C11F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3755,21 +3757,21 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.41015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="18.234375" customWidth="1"/>
-    <col min="6" max="8" width="14.76171875" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="6" max="8" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C1" s="24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C4" s="27"/>
       <c r="D4" s="133" t="s">
         <v>18</v>
@@ -3780,7 +3782,7 @@
       </c>
       <c r="G4" s="133"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="10"/>
       <c r="C5" s="28" t="s">
         <v>20</v>
@@ -3801,7 +3803,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="10">
         <v>5</v>
       </c>
@@ -3823,7 +3825,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="10">
         <v>1</v>
       </c>
@@ -3851,7 +3853,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="10">
         <v>2</v>
       </c>
@@ -3879,7 +3881,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="10">
         <v>3</v>
       </c>
@@ -3907,7 +3909,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="10">
         <v>4</v>
       </c>
@@ -3935,7 +3937,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="10"/>
       <c r="C11" s="17" t="s">
         <v>27</v>
@@ -3955,10 +3957,10 @@
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D12" s="4"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C14" s="27"/>
       <c r="D14" s="133" t="s">
         <v>28</v>
@@ -3966,7 +3968,7 @@
       <c r="E14" s="133"/>
       <c r="F14" s="27"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C15" s="27" t="s">
         <v>29</v>
       </c>
@@ -3980,7 +3982,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>1</v>
       </c>
@@ -4000,7 +4002,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>2</v>
       </c>
@@ -4020,7 +4022,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>3</v>
       </c>
@@ -4040,7 +4042,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>4</v>
       </c>
@@ -4060,7 +4062,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>5</v>
       </c>
@@ -4080,7 +4082,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>6</v>
       </c>
@@ -4100,7 +4102,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>7</v>
       </c>
@@ -4120,7 +4122,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>8</v>
       </c>
@@ -4140,7 +4142,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>9</v>
       </c>
@@ -4160,7 +4162,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>10</v>
       </c>
@@ -4180,7 +4182,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>11</v>
       </c>
@@ -4200,7 +4202,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>12</v>
       </c>
@@ -4214,7 +4216,7 @@
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C28" s="20"/>
     </row>
   </sheetData>
@@ -4259,22 +4261,22 @@
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.41015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="18.234375" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.76171875" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C1" s="24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:8" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="29"/>
       <c r="C3" s="28" t="s">
         <v>43</v>
@@ -4295,7 +4297,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="10">
         <v>0</v>
       </c>
@@ -4314,7 +4316,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="10">
         <v>1</v>
       </c>
@@ -4342,7 +4344,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="10">
         <v>2</v>
       </c>
@@ -4370,7 +4372,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="10">
         <v>3</v>
       </c>
@@ -4398,7 +4400,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="10">
         <v>4</v>
       </c>
@@ -4426,7 +4428,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="24" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="17"/>
       <c r="C9" s="17" t="s">
         <v>27</v>
@@ -4443,7 +4445,7 @@
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C12" s="27"/>
       <c r="D12" s="133" t="s">
         <v>50</v>
@@ -4451,7 +4453,7 @@
       <c r="E12" s="133"/>
       <c r="F12" s="27"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C13" s="27" t="s">
         <v>29</v>
       </c>
@@ -4465,7 +4467,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>1</v>
       </c>
@@ -4485,7 +4487,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>2</v>
       </c>
@@ -4505,7 +4507,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>3</v>
       </c>
@@ -4525,7 +4527,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>4</v>
       </c>
@@ -4545,7 +4547,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>5</v>
       </c>
@@ -4565,7 +4567,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>6</v>
       </c>
@@ -4585,7 +4587,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>7</v>
       </c>
@@ -4605,7 +4607,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>8</v>
       </c>
@@ -4625,7 +4627,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>9</v>
       </c>
@@ -4645,7 +4647,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>10</v>
       </c>
@@ -4665,7 +4667,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>11</v>
       </c>
@@ -4685,7 +4687,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>12</v>
       </c>
@@ -4699,7 +4701,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C26" s="52" t="s">
         <v>27</v>
       </c>
@@ -4713,7 +4715,7 @@
       </c>
       <c r="F26" s="17"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="D28" s="4"/>
     </row>
   </sheetData>
@@ -4756,20 +4758,20 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="8.87890625" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="8.90625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="14.41015625" customWidth="1"/>
-    <col min="6" max="6" width="15.234375" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D2" s="24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D5" s="53"/>
       <c r="E5" s="48" t="s">
         <v>2</v>
@@ -4778,7 +4780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D6" s="56" t="s">
         <v>52</v>
       </c>
@@ -4789,12 +4791,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D7" s="49" t="s">
         <v>56</v>
@@ -4809,12 +4811,12 @@
       </c>
       <c r="G7" s="123"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D8" s="46" t="s">
         <v>58</v>
@@ -4829,12 +4831,12 @@
       </c>
       <c r="G8" s="123"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>33</v>
@@ -4849,7 +4851,7 @@
       </c>
       <c r="G9" s="123"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D10" s="54" t="s">
         <v>27</v>
       </c>
@@ -4876,30 +4878,30 @@
       <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.234375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.52734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.87890625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.76171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.41015625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.36328125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="10" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.76171875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.76171875" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7265625" style="3" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.76171875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C1" s="24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C2" s="24"/>
     </row>
-    <row r="4" spans="2:13" s="24" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:13" s="24" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="25" t="s">
         <v>61</v>
       </c>
@@ -4930,7 +4932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="26" t="s">
         <v>67</v>
       </c>
@@ -4968,7 +4970,7 @@
       </c>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6" s="26" t="s">
         <v>69</v>
       </c>
@@ -5006,7 +5008,7 @@
       </c>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7" s="26" t="s">
         <v>71</v>
       </c>
@@ -5044,7 +5046,7 @@
       </c>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8" s="26" t="s">
         <v>73</v>
       </c>
@@ -5082,7 +5084,7 @@
       </c>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" s="26" t="s">
         <v>75</v>
       </c>
@@ -5120,7 +5122,7 @@
       </c>
       <c r="M9" s="5"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="26" t="s">
         <v>77</v>
       </c>
@@ -5158,7 +5160,7 @@
       </c>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" s="26" t="s">
         <v>79</v>
       </c>
@@ -5196,7 +5198,7 @@
       </c>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12" s="26" t="s">
         <v>81</v>
       </c>
@@ -5234,7 +5236,7 @@
       </c>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B13" s="26" t="s">
         <v>83</v>
       </c>
@@ -5272,7 +5274,7 @@
       </c>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B14" s="26" t="s">
         <v>85</v>
       </c>
@@ -5310,7 +5312,7 @@
       </c>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B15" s="26" t="s">
         <v>87</v>
       </c>
@@ -5348,7 +5350,7 @@
       </c>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16" s="26" t="s">
         <v>89</v>
       </c>
@@ -5386,7 +5388,7 @@
       </c>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B17" s="26" t="s">
         <v>91</v>
       </c>
@@ -5424,7 +5426,7 @@
       </c>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B18" s="26" t="s">
         <v>93</v>
       </c>
@@ -5462,7 +5464,7 @@
       </c>
       <c r="M18" s="5"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B19" s="26" t="s">
         <v>95</v>
       </c>
@@ -5500,7 +5502,7 @@
       </c>
       <c r="M19" s="5"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B20" s="26" t="s">
         <v>97</v>
       </c>
@@ -5538,7 +5540,7 @@
       </c>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B21" s="26" t="s">
         <v>99</v>
       </c>
@@ -5576,7 +5578,7 @@
       </c>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B22" s="26" t="s">
         <v>101</v>
       </c>
@@ -5614,7 +5616,7 @@
       </c>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B23" s="26" t="s">
         <v>103</v>
       </c>
@@ -5652,7 +5654,7 @@
       </c>
       <c r="M23" s="5"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B24" s="26" t="s">
         <v>105</v>
       </c>
@@ -5690,7 +5692,7 @@
       </c>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B25" s="26" t="s">
         <v>107</v>
       </c>
@@ -5728,7 +5730,7 @@
       </c>
       <c r="M25" s="5"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="6" t="s">
         <v>27</v>
@@ -5761,12 +5763,12 @@
       </c>
       <c r="M26" s="5"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C29" s="59" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="C30" s="30" t="s">
         <v>110</v>
       </c>
@@ -5794,7 +5796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C31" s="10" t="s">
         <v>111</v>
       </c>
@@ -5826,7 +5828,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C32" s="10" t="s">
         <v>112</v>
       </c>
@@ -5858,7 +5860,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C33" s="10" t="s">
         <v>6</v>
       </c>
@@ -5890,7 +5892,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="24" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="3:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C34" s="17" t="s">
         <v>27</v>
       </c>
@@ -5922,11 +5924,11 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
       <c r="K35" s="12"/>
       <c r="L35" s="13"/>
     </row>
-    <row r="36" spans="3:12" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="36" spans="3:12" ht="29" x14ac:dyDescent="0.35">
       <c r="C36" s="30" t="s">
         <v>113</v>
       </c>
@@ -5954,7 +5956,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C37" s="10" t="s">
         <v>114</v>
       </c>
@@ -5986,7 +5988,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C38" s="10" t="s">
         <v>115</v>
       </c>
@@ -6018,7 +6020,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C39" s="10" t="s">
         <v>116</v>
       </c>
@@ -6050,7 +6052,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C40" s="10" t="s">
         <v>117</v>
       </c>
@@ -6082,7 +6084,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="3:12" s="24" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="3:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C41" s="17" t="s">
         <v>27</v>
       </c>
@@ -6114,11 +6116,11 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
       <c r="K42" s="12"/>
       <c r="L42" s="13"/>
     </row>
-    <row r="43" spans="3:12" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="43" spans="3:12" ht="29" x14ac:dyDescent="0.35">
       <c r="C43" s="30" t="s">
         <v>118</v>
       </c>
@@ -6146,7 +6148,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C44" s="10" t="s">
         <v>119</v>
       </c>
@@ -6178,7 +6180,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C45" s="10" t="s">
         <v>120</v>
       </c>
@@ -6210,7 +6212,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="46" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C46" s="10" t="s">
         <v>121</v>
       </c>
@@ -6242,7 +6244,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="3:12" s="24" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="3:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C47" s="17" t="s">
         <v>27</v>
       </c>
@@ -6296,24 +6298,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D685E9F-E32C-412F-B12B-43F1DB44B054}">
   <dimension ref="B1:L51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.41015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.76171875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.52734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.41015625" customWidth="1"/>
-    <col min="11" max="11" width="14.76171875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.41015625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.36328125" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
       <c r="D1" s="47" t="s">
@@ -6321,7 +6323,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" s="17" t="s">
         <v>122</v>
       </c>
@@ -6335,10 +6337,10 @@
         <v>125</v>
       </c>
       <c r="G2" s="117" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.5">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -6362,7 +6364,7 @@
       </c>
       <c r="K3" s="135"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="10">
         <v>2</v>
       </c>
@@ -6378,25 +6380,25 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G4" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="H4" s="118" t="s">
+      <c r="I4" s="119" t="s">
         <v>128</v>
       </c>
-      <c r="I4" s="119" t="s">
+      <c r="J4" s="119" t="s">
         <v>129</v>
       </c>
-      <c r="J4" s="119" t="s">
+      <c r="K4" s="119" t="s">
         <v>130</v>
-      </c>
-      <c r="K4" s="119" t="s">
-        <v>131</v>
       </c>
       <c r="L4" s="84" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="10">
         <v>3</v>
       </c>
@@ -6412,7 +6414,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H5" s="114">
         <f>SUMIFS(ModelData!BE:BE,ModelData!BD:BD,'Route Start Time'!G5)</f>
@@ -6434,7 +6436,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="10">
         <v>4</v>
       </c>
@@ -6450,7 +6452,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H6" s="114">
         <f>SUMIFS(ModelData!BE:BE,ModelData!BD:BD,'Route Start Time'!G6)</f>
@@ -6472,7 +6474,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="10">
         <v>5</v>
       </c>
@@ -6488,7 +6490,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H7" s="114">
         <f>SUMIFS(ModelData!BE:BE,ModelData!BD:BD,'Route Start Time'!G7)</f>
@@ -6510,7 +6512,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="10">
         <v>6</v>
       </c>
@@ -6526,7 +6528,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H8" s="114">
         <f>SUMIFS(ModelData!BE:BE,ModelData!BD:BD,'Route Start Time'!G8)</f>
@@ -6548,7 +6550,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="10">
         <v>7</v>
       </c>
@@ -6564,7 +6566,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H9" s="114">
         <f>SUMIFS(ModelData!BE:BE,ModelData!BD:BD,'Route Start Time'!G9)</f>
@@ -6586,7 +6588,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="10">
         <v>8</v>
       </c>
@@ -6625,7 +6627,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="10">
         <v>9</v>
       </c>
@@ -6641,7 +6643,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="10">
         <v>10</v>
       </c>
@@ -6657,7 +6659,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="10">
         <v>11</v>
       </c>
@@ -6673,7 +6675,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="10">
         <v>12</v>
       </c>
@@ -6689,10 +6691,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G14" s="117" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.5">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="10">
         <v>13</v>
       </c>
@@ -6716,7 +6718,7 @@
       </c>
       <c r="K15" s="137"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="10">
         <v>14</v>
       </c>
@@ -6732,25 +6734,25 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G16" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="H16" s="118" t="s">
+      <c r="I16" s="119" t="s">
         <v>128</v>
       </c>
-      <c r="I16" s="119" t="s">
+      <c r="J16" s="120" t="s">
         <v>129</v>
       </c>
-      <c r="J16" s="120" t="s">
+      <c r="K16" s="119" t="s">
         <v>130</v>
-      </c>
-      <c r="K16" s="119" t="s">
-        <v>131</v>
       </c>
       <c r="L16" s="84" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -6766,7 +6768,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H17" s="114" t="e">
         <f>VLOOKUP(G17,ModelData!EB:EC,2,FALSE)</f>
@@ -6789,7 +6791,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="10">
         <v>16</v>
       </c>
@@ -6805,7 +6807,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H18" s="114" t="e">
         <f>VLOOKUP(G18,ModelData!EB:EC,2,FALSE)</f>
@@ -6828,7 +6830,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="10">
         <v>17</v>
       </c>
@@ -6844,7 +6846,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H19" s="114" t="e">
         <f>VLOOKUP(G19,ModelData!EB:EC,2,FALSE)</f>
@@ -6867,7 +6869,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="10">
         <v>18</v>
       </c>
@@ -6883,7 +6885,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H20" s="114" t="e">
         <f>VLOOKUP(G20,ModelData!EB:EC,2,FALSE)</f>
@@ -6906,7 +6908,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="10">
         <v>19</v>
       </c>
@@ -6922,7 +6924,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H21" s="114" t="e">
         <f>VLOOKUP(G21,ModelData!EB:EC,2,FALSE)</f>
@@ -6945,7 +6947,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="10">
         <v>20</v>
       </c>
@@ -6984,7 +6986,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="10">
         <v>21</v>
       </c>
@@ -7000,7 +7002,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="10">
         <v>22</v>
       </c>
@@ -7017,7 +7019,7 @@
       </c>
       <c r="H24"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="10">
         <v>23</v>
       </c>
@@ -7036,7 +7038,7 @@
       <c r="J25" s="64"/>
       <c r="K25" s="76"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="10">
         <v>24</v>
       </c>
@@ -7055,7 +7057,7 @@
       <c r="J26" s="64"/>
       <c r="K26" s="64"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="10">
         <v>25</v>
       </c>
@@ -7074,7 +7076,7 @@
       <c r="J27" s="64"/>
       <c r="K27" s="76"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="10">
         <v>26</v>
       </c>
@@ -7093,7 +7095,7 @@
       <c r="J28" s="64"/>
       <c r="K28" s="76"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" s="10">
         <v>27</v>
       </c>
@@ -7112,7 +7114,7 @@
       <c r="J29" s="64"/>
       <c r="K29" s="76"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="10">
         <v>28</v>
       </c>
@@ -7129,7 +7131,7 @@
       </c>
       <c r="H30"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" s="10">
         <v>29</v>
       </c>
@@ -7145,7 +7147,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="10">
         <v>30</v>
       </c>
@@ -7161,7 +7163,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="10">
         <v>31</v>
       </c>
@@ -7177,7 +7179,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="10">
         <v>32</v>
       </c>
@@ -7193,7 +7195,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="10">
         <v>33</v>
       </c>
@@ -7209,7 +7211,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="10">
         <v>34</v>
       </c>
@@ -7225,7 +7227,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="10">
         <v>35</v>
       </c>
@@ -7241,7 +7243,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="10">
         <v>36</v>
       </c>
@@ -7257,7 +7259,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="10">
         <v>37</v>
       </c>
@@ -7273,7 +7275,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="10">
         <v>38</v>
       </c>
@@ -7289,7 +7291,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="10">
         <v>39</v>
       </c>
@@ -7305,7 +7307,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" s="10">
         <v>40</v>
       </c>
@@ -7321,7 +7323,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" s="10">
         <v>41</v>
       </c>
@@ -7337,7 +7339,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B44" s="10">
         <v>42</v>
       </c>
@@ -7353,7 +7355,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B45" s="10">
         <v>43</v>
       </c>
@@ -7369,7 +7371,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B46" s="10">
         <v>44</v>
       </c>
@@ -7385,7 +7387,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B47" s="10">
         <v>45</v>
       </c>
@@ -7401,7 +7403,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B48" s="10">
         <v>46</v>
       </c>
@@ -7417,7 +7419,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" s="10">
         <v>47</v>
       </c>
@@ -7433,7 +7435,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" s="10">
         <v>48</v>
       </c>
@@ -7449,7 +7451,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" s="17"/>
       <c r="C51" s="17" t="s">
         <v>27</v>
@@ -7540,36 +7542,36 @@
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.76171875" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.234375" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.76171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.41015625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="133" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E3" s="133"/>
       <c r="F3" s="133" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G3" s="133"/>
       <c r="H3" s="27"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>2</v>
@@ -7587,12 +7589,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D5" s="7">
         <f>SUMIFS(ModelData!BP:BP,ModelData!BN:BN,'Route OriginationTerminal'!B5)</f>
@@ -7615,12 +7617,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D6" s="7">
         <f>SUMIFS(ModelData!BP:BP,ModelData!BN:BN,'Route OriginationTerminal'!B6)</f>
@@ -7643,9 +7645,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>115</v>
@@ -7671,12 +7673,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D8" s="7">
         <f>SUMIFS(ModelData!BP:BP,ModelData!BN:BN,'Route OriginationTerminal'!B8)</f>
@@ -7699,7 +7701,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="17"/>
       <c r="C9" s="17" t="s">
         <v>27</v>
@@ -7716,23 +7718,23 @@
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="27" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="133" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E11" s="133"/>
       <c r="F11" s="27"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>2</v>
@@ -7744,12 +7746,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D13" s="62">
         <f>SUMIFS(ModelData!BY:BY,ModelData!BX:BX,'Route OriginationTerminal'!B13)</f>
@@ -7764,9 +7766,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>115</v>
@@ -7784,12 +7786,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D15" s="62">
         <f>SUMIFS(ModelData!BY:BY,ModelData!BX:BX,'Route OriginationTerminal'!B15)</f>
@@ -7804,9 +7806,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19" s="27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="29"/>
@@ -7815,12 +7817,12 @@
       <c r="G19" s="29"/>
       <c r="H19" s="29"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D20" s="27" t="s">
         <v>2</v>
@@ -7838,12 +7840,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D21" s="7">
         <f>SUMIFS(ModelData!CF:CF,ModelData!CD:CD,'Route OriginationTerminal'!B21)</f>
@@ -7866,12 +7868,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D22" s="7">
         <f>SUMIFS(ModelData!CF:CF,ModelData!CD:CD,'Route OriginationTerminal'!B22)</f>
@@ -7894,9 +7896,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>115</v>
@@ -7922,12 +7924,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D24" s="7">
         <f>SUMIFS(ModelData!CF:CF,ModelData!CD:CD,'Route OriginationTerminal'!B24)</f>
@@ -7950,7 +7952,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="17"/>
       <c r="C25" s="17" t="s">
         <v>27</v>
@@ -7967,32 +7969,32 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" s="27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
       <c r="F28" s="29"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="133" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E29" s="133"/>
       <c r="F29" s="27"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D30" s="27" t="s">
         <v>2</v>
@@ -8004,12 +8006,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B31" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D31" s="62">
         <f>SUMIFS(ModelData!CO:CO,ModelData!CN:CN,'Route OriginationTerminal'!B31)</f>
@@ -8024,9 +8026,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>115</v>
@@ -8044,12 +8046,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B33" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D33" s="62">
         <f>SUMIFS(ModelData!CO:CO,ModelData!CN:CN,'Route OriginationTerminal'!B33)</f>
@@ -8131,35 +8133,35 @@
       <selection activeCell="AF55" sqref="AF55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.41015625" customWidth="1"/>
-    <col min="2" max="2" width="17.76171875" customWidth="1"/>
-    <col min="3" max="3" width="17.41015625" customWidth="1"/>
-    <col min="4" max="4" width="10.41015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.76171875" customWidth="1"/>
-    <col min="6" max="6" width="10.87890625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.3515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.41015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.41015625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.76171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.234375" customWidth="1"/>
-    <col min="28" max="28" width="18.234375" customWidth="1"/>
-    <col min="29" max="29" width="11.76171875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.41015625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.76171875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.76171875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.41015625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.26953125" customWidth="1"/>
+    <col min="28" max="28" width="18.26953125" customWidth="1"/>
+    <col min="29" max="29" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="23.35" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:33" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="138" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="140" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D1" s="140"/>
       <c r="E1" s="140"/>
@@ -8182,10 +8184,10 @@
       <c r="V1" s="140"/>
       <c r="W1" s="140"/>
       <c r="AB1" s="93" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="138"/>
       <c r="B2" s="64"/>
       <c r="C2" s="64"/>
@@ -8226,96 +8228,96 @@
       <c r="V2" s="64"/>
       <c r="W2" s="64"/>
     </row>
-    <row r="3" spans="1:33" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="138"/>
       <c r="B3" s="139" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="109" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="63" t="s">
         <v>157</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="F3" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="E3" s="63" t="s">
+      <c r="G3" s="63" t="s">
         <v>159</v>
       </c>
-      <c r="F3" s="63" t="s">
+      <c r="H3" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="I3" s="63" t="s">
         <v>161</v>
-      </c>
-      <c r="H3" s="63" t="s">
-        <v>162</v>
-      </c>
-      <c r="I3" s="63" t="s">
-        <v>163</v>
       </c>
       <c r="J3" s="63" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="63" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L3" s="66" t="s">
         <v>27</v>
       </c>
       <c r="M3" s="64"/>
       <c r="N3" s="110" t="s">
+        <v>156</v>
+      </c>
+      <c r="O3" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="P3" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q3" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="O3" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="P3" s="63" t="s">
+      <c r="R3" s="63" t="s">
         <v>159</v>
       </c>
-      <c r="Q3" s="63" t="s">
+      <c r="S3" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="R3" s="63" t="s">
+      <c r="T3" s="63" t="s">
         <v>161</v>
-      </c>
-      <c r="S3" s="63" t="s">
-        <v>162</v>
-      </c>
-      <c r="T3" s="63" t="s">
-        <v>163</v>
       </c>
       <c r="U3" s="63" t="s">
         <v>6</v>
       </c>
       <c r="V3" s="63" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="W3" s="66" t="s">
         <v>27</v>
       </c>
       <c r="AB3" s="84" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AC3" s="84" t="s">
         <v>2</v>
       </c>
       <c r="AD3" s="84" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AE3" s="84" t="s">
         <v>3</v>
       </c>
       <c r="AF3" s="84" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AG3" s="84" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="138"/>
       <c r="B4" s="139"/>
       <c r="C4" s="68" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D4" s="128" t="e">
         <f>VLOOKUP($C4,SurveyData!$CS:$DA,D$2,FALSE)</f>
@@ -8355,7 +8357,7 @@
       </c>
       <c r="M4" s="64"/>
       <c r="N4" s="71" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O4" s="72">
         <f>IFERROR(D4/$L$12,0)</f>
@@ -8394,7 +8396,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="84" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC4" s="82" t="e">
         <f>VLOOKUP(AB4,ModelData!DD:DE,2,FALSE)</f>
@@ -8417,11 +8419,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="138"/>
       <c r="B5" s="139"/>
       <c r="C5" s="68" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D5" s="128" t="e">
         <f>VLOOKUP($C5,SurveyData!$CS:$DA,D$2,FALSE)</f>
@@ -8461,7 +8463,7 @@
       </c>
       <c r="M5" s="64"/>
       <c r="N5" s="71" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O5" s="72">
         <f t="shared" ref="O5:O12" si="2">IFERROR(D5/$L$12,0)</f>
@@ -8500,7 +8502,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="84" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC5" s="82" t="e">
         <f>VLOOKUP(AB5,ModelData!DD:DE,2,FALSE)</f>
@@ -8523,11 +8525,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="138"/>
       <c r="B6" s="139"/>
       <c r="C6" s="68" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D6" s="128" t="e">
         <f>VLOOKUP($C6,SurveyData!$CS:$DA,D$2,FALSE)</f>
@@ -8567,7 +8569,7 @@
       </c>
       <c r="M6" s="64"/>
       <c r="N6" s="71" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O6" s="72">
         <f t="shared" si="2"/>
@@ -8606,7 +8608,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AC6" s="82" t="e">
         <f>VLOOKUP(AB6,ModelData!DD:DE,2,FALSE)</f>
@@ -8629,11 +8631,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="138"/>
       <c r="B7" s="139"/>
       <c r="C7" s="68" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D7" s="128" t="e">
         <f>VLOOKUP($C7,SurveyData!$CS:$DA,D$2,FALSE)</f>
@@ -8673,7 +8675,7 @@
       </c>
       <c r="M7" s="64"/>
       <c r="N7" s="71" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O7" s="72">
         <f t="shared" si="2"/>
@@ -8712,7 +8714,7 @@
         <v>0</v>
       </c>
       <c r="AB7" s="84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AC7" s="82" t="e">
         <f>VLOOKUP(AB7,ModelData!DD:DE,2,FALSE)</f>
@@ -8735,11 +8737,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" s="138"/>
       <c r="B8" s="139"/>
       <c r="C8" s="68" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D8" s="128" t="e">
         <f>VLOOKUP($C8,SurveyData!$CS:$DA,D$2,FALSE)</f>
@@ -8779,7 +8781,7 @@
       </c>
       <c r="M8" s="64"/>
       <c r="N8" s="71" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O8" s="72">
         <f t="shared" si="2"/>
@@ -8818,7 +8820,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="84" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AC8" s="82" t="e">
         <f>VLOOKUP(AB8,ModelData!DD:DE,2,FALSE)</f>
@@ -8841,11 +8843,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="138"/>
       <c r="B9" s="139"/>
       <c r="C9" s="68" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D9" s="128" t="e">
         <f>VLOOKUP($C9,SurveyData!$CS:$DA,D$2,FALSE)</f>
@@ -8885,7 +8887,7 @@
       </c>
       <c r="M9" s="64"/>
       <c r="N9" s="71" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="O9" s="72">
         <f t="shared" si="2"/>
@@ -8944,7 +8946,7 @@
       </c>
       <c r="AG9" s="84"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="138"/>
       <c r="B10" s="139"/>
       <c r="C10" s="68" t="s">
@@ -8988,7 +8990,7 @@
       </c>
       <c r="M10" s="64"/>
       <c r="N10" s="71" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O10" s="72">
         <f t="shared" si="2"/>
@@ -9027,11 +9029,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="138"/>
       <c r="B11" s="139"/>
       <c r="C11" s="68" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D11" s="128" t="e">
         <f>VLOOKUP($C11,SurveyData!$CS:$DA,D$2,FALSE)</f>
@@ -9066,11 +9068,11 @@
         <v>#N/A</v>
       </c>
       <c r="L11" s="77" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M11" s="64"/>
       <c r="N11" s="71" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O11" s="72">
         <f t="shared" si="2"/>
@@ -9109,7 +9111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="138"/>
       <c r="B12" s="139"/>
       <c r="C12" s="66" t="s">
@@ -9192,7 +9194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="138"/>
       <c r="B13" s="64"/>
       <c r="C13" s="64"/>
@@ -9217,7 +9219,7 @@
       <c r="V13" s="64"/>
       <c r="W13" s="64"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="138"/>
       <c r="B14" s="64"/>
       <c r="C14" s="64"/>
@@ -9242,7 +9244,7 @@
       <c r="V14" s="64"/>
       <c r="W14" s="64"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="138"/>
       <c r="B15" s="64"/>
       <c r="C15" s="64"/>
@@ -9267,78 +9269,78 @@
       <c r="V15" s="64"/>
       <c r="W15" s="64"/>
     </row>
-    <row r="16" spans="1:33" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="138"/>
       <c r="B16" s="139" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="109" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="F16" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="C16" s="109" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" s="63" t="s">
-        <v>143</v>
-      </c>
-      <c r="E16" s="63" t="s">
+      <c r="G16" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="F16" s="63" t="s">
+      <c r="H16" s="63" t="s">
         <v>171</v>
       </c>
-      <c r="G16" s="63" t="s">
+      <c r="I16" s="63" t="s">
         <v>172</v>
       </c>
-      <c r="H16" s="63" t="s">
+      <c r="J16" s="63" t="s">
         <v>173</v>
       </c>
-      <c r="I16" s="63" t="s">
+      <c r="K16" s="63" t="s">
         <v>174</v>
-      </c>
-      <c r="J16" s="63" t="s">
-        <v>175</v>
-      </c>
-      <c r="K16" s="63" t="s">
-        <v>176</v>
       </c>
       <c r="L16" s="66" t="s">
         <v>27</v>
       </c>
       <c r="M16" s="64"/>
       <c r="N16" s="110" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O16" s="63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P16" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q16" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="R16" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="Q16" s="63" t="s">
+      <c r="S16" s="63" t="s">
         <v>171</v>
       </c>
-      <c r="R16" s="63" t="s">
+      <c r="T16" s="63" t="s">
         <v>172</v>
       </c>
-      <c r="S16" s="63" t="s">
+      <c r="U16" s="63" t="s">
         <v>173</v>
       </c>
-      <c r="T16" s="63" t="s">
+      <c r="V16" s="63" t="s">
         <v>174</v>
-      </c>
-      <c r="U16" s="63" t="s">
-        <v>175</v>
-      </c>
-      <c r="V16" s="63" t="s">
-        <v>176</v>
       </c>
       <c r="W16" s="66" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="138"/>
       <c r="B17" s="139"/>
       <c r="C17" s="68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D17" s="69" t="e">
         <f>VLOOKUP($C17,ModelData!$CS:$DA,D$2,FALSE)</f>
@@ -9378,7 +9380,7 @@
       </c>
       <c r="M17" s="64"/>
       <c r="N17" s="68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="O17" s="73">
         <f>IFERROR(D17/$L$25,0)</f>
@@ -9417,11 +9419,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="138"/>
       <c r="B18" s="139"/>
       <c r="C18" s="68" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D18" s="69" t="e">
         <f>VLOOKUP($C18,ModelData!$CS:$DA,D$2,FALSE)</f>
@@ -9461,7 +9463,7 @@
       </c>
       <c r="M18" s="64"/>
       <c r="N18" s="68" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O18" s="73">
         <f t="shared" ref="O18:O25" si="17">IFERROR(D18/$L$25,0)</f>
@@ -9500,11 +9502,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="138"/>
       <c r="B19" s="139"/>
       <c r="C19" s="68" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D19" s="69" t="e">
         <f>VLOOKUP($C19,ModelData!$CS:$DA,D$2,FALSE)</f>
@@ -9544,7 +9546,7 @@
       </c>
       <c r="M19" s="64"/>
       <c r="N19" s="68" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="O19" s="73">
         <f t="shared" si="17"/>
@@ -9583,11 +9585,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="138"/>
       <c r="B20" s="139"/>
       <c r="C20" s="68" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D20" s="69" t="e">
         <f>VLOOKUP($C20,ModelData!$CS:$DA,D$2,FALSE)</f>
@@ -9627,7 +9629,7 @@
       </c>
       <c r="M20" s="64"/>
       <c r="N20" s="68" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="O20" s="73">
         <f t="shared" si="17"/>
@@ -9666,11 +9668,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="138"/>
       <c r="B21" s="139"/>
       <c r="C21" s="68" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D21" s="69" t="e">
         <f>VLOOKUP($C21,ModelData!$CS:$DA,D$2,FALSE)</f>
@@ -9710,7 +9712,7 @@
       </c>
       <c r="M21" s="64"/>
       <c r="N21" s="68" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="O21" s="73">
         <f t="shared" si="17"/>
@@ -9749,11 +9751,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="138"/>
       <c r="B22" s="139"/>
       <c r="C22" s="68" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D22" s="69" t="e">
         <f>VLOOKUP($C22,ModelData!$CS:$DA,D$2,FALSE)</f>
@@ -9793,7 +9795,7 @@
       </c>
       <c r="M22" s="64"/>
       <c r="N22" s="68" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="O22" s="73">
         <f t="shared" si="17"/>
@@ -9832,11 +9834,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="138"/>
       <c r="B23" s="139"/>
       <c r="C23" s="68" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D23" s="69" t="e">
         <f>VLOOKUP($C23,ModelData!$CS:$DA,D$2,FALSE)</f>
@@ -9876,7 +9878,7 @@
       </c>
       <c r="M23" s="64"/>
       <c r="N23" s="68" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="O23" s="73">
         <f t="shared" si="17"/>
@@ -9915,11 +9917,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="138"/>
       <c r="B24" s="139"/>
       <c r="C24" s="68" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D24" s="69" t="e">
         <f>VLOOKUP($C24,ModelData!$CS:$DA,D$2,FALSE)</f>
@@ -9959,7 +9961,7 @@
       </c>
       <c r="M24" s="64"/>
       <c r="N24" s="68" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="O24" s="73">
         <f t="shared" si="17"/>
@@ -9998,7 +10000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="138"/>
       <c r="B25" s="139"/>
       <c r="C25" s="66" t="s">
@@ -10081,7 +10083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="138"/>
       <c r="B26" s="64"/>
       <c r="C26" s="64"/>
@@ -10106,7 +10108,7 @@
       <c r="V26" s="64"/>
       <c r="W26" s="64"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="138"/>
       <c r="B27" s="64"/>
       <c r="C27" s="64"/>
@@ -10131,7 +10133,7 @@
       <c r="V27" s="64"/>
       <c r="W27" s="64"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="138"/>
       <c r="B28" s="64"/>
       <c r="C28" s="64"/>
@@ -10156,7 +10158,7 @@
       <c r="V28" s="64"/>
       <c r="W28" s="64"/>
     </row>
-    <row r="29" spans="1:23" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:23" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="138"/>
       <c r="B29" s="64"/>
       <c r="C29" s="64"/>
@@ -10171,37 +10173,37 @@
       <c r="L29" s="141"/>
       <c r="M29" s="64"/>
       <c r="N29" s="111" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O29" s="78" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P29" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q29" s="78" t="s">
+        <v>169</v>
+      </c>
+      <c r="R29" s="78" t="s">
         <v>170</v>
       </c>
-      <c r="Q29" s="78" t="s">
+      <c r="S29" s="78" t="s">
         <v>171</v>
       </c>
-      <c r="R29" s="78" t="s">
+      <c r="T29" s="78" t="s">
         <v>172</v>
       </c>
-      <c r="S29" s="78" t="s">
+      <c r="U29" s="78" t="s">
         <v>173</v>
       </c>
-      <c r="T29" s="78" t="s">
+      <c r="V29" s="78" t="s">
         <v>174</v>
-      </c>
-      <c r="U29" s="78" t="s">
-        <v>175</v>
-      </c>
-      <c r="V29" s="78" t="s">
-        <v>176</v>
       </c>
       <c r="W29" s="79" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="138"/>
       <c r="B30" s="64"/>
       <c r="C30" s="64"/>
@@ -10216,7 +10218,7 @@
       <c r="L30" s="141"/>
       <c r="M30" s="64"/>
       <c r="N30" s="79" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="O30" s="81">
         <f>O17-O4</f>
@@ -10255,7 +10257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="138"/>
       <c r="B31" s="64"/>
       <c r="C31" s="64"/>
@@ -10270,7 +10272,7 @@
       <c r="L31" s="141"/>
       <c r="M31" s="64"/>
       <c r="N31" s="79" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O31" s="81">
         <f t="shared" ref="O31:W31" si="28">O18-O5</f>
@@ -10309,7 +10311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="138"/>
       <c r="B32" s="64"/>
       <c r="C32" s="64"/>
@@ -10324,7 +10326,7 @@
       <c r="L32" s="141"/>
       <c r="M32" s="64"/>
       <c r="N32" s="79" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="O32" s="81">
         <f t="shared" ref="O32:W32" si="29">O19-O6</f>
@@ -10363,7 +10365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A33" s="138"/>
       <c r="B33" s="64"/>
       <c r="C33" s="64"/>
@@ -10378,7 +10380,7 @@
       <c r="L33" s="141"/>
       <c r="M33" s="64"/>
       <c r="N33" s="79" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="O33" s="81">
         <f t="shared" ref="O33:W33" si="30">O20-O7</f>
@@ -10417,7 +10419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A34" s="138"/>
       <c r="B34" s="64"/>
       <c r="C34" s="64"/>
@@ -10432,7 +10434,7 @@
       <c r="L34" s="141"/>
       <c r="M34" s="64"/>
       <c r="N34" s="79" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="O34" s="81">
         <f t="shared" ref="O34:W34" si="31">O21-O8</f>
@@ -10471,7 +10473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A35" s="138"/>
       <c r="B35" s="64"/>
       <c r="C35" s="64"/>
@@ -10486,7 +10488,7 @@
       <c r="L35" s="141"/>
       <c r="M35" s="64"/>
       <c r="N35" s="79" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="O35" s="81">
         <f t="shared" ref="O35:W35" si="32">O22-O9</f>
@@ -10525,7 +10527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A36" s="138"/>
       <c r="B36" s="64"/>
       <c r="C36" s="64"/>
@@ -10540,7 +10542,7 @@
       <c r="L36" s="141"/>
       <c r="M36" s="64"/>
       <c r="N36" s="79" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="O36" s="81">
         <f t="shared" ref="O36:W36" si="33">O23-O10</f>
@@ -10579,7 +10581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A37" s="138"/>
       <c r="B37" s="64"/>
       <c r="C37" s="64"/>
@@ -10594,7 +10596,7 @@
       <c r="L37" s="141"/>
       <c r="M37" s="64"/>
       <c r="N37" s="79" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="O37" s="81">
         <f t="shared" ref="O37:W37" si="34">O24-O11</f>
@@ -10633,7 +10635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A38" s="138"/>
       <c r="B38" s="64"/>
       <c r="C38" s="64"/>
@@ -10687,10 +10689,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="23.35" x14ac:dyDescent="0.8">
+    <row r="43" spans="1:33" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="64"/>
       <c r="C43" s="140" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D43" s="140"/>
       <c r="E43" s="140"/>
@@ -10713,10 +10715,10 @@
       <c r="V43" s="140"/>
       <c r="W43" s="140"/>
       <c r="AB43" s="93" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.5">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
       <c r="D44">
         <v>2</v>
       </c>
@@ -10742,98 +10744,98 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:33" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A45" s="138" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B45" s="139" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="112" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="97" t="s">
+        <v>142</v>
+      </c>
+      <c r="E45" s="97" t="s">
+        <v>157</v>
+      </c>
+      <c r="F45" s="97" t="s">
         <v>158</v>
       </c>
-      <c r="D45" s="97" t="s">
-        <v>144</v>
-      </c>
-      <c r="E45" s="97" t="s">
+      <c r="G45" s="97" t="s">
         <v>159</v>
       </c>
-      <c r="F45" s="97" t="s">
+      <c r="H45" s="97" t="s">
         <v>160</v>
       </c>
-      <c r="G45" s="97" t="s">
+      <c r="I45" s="97" t="s">
         <v>161</v>
-      </c>
-      <c r="H45" s="97" t="s">
-        <v>162</v>
-      </c>
-      <c r="I45" s="97" t="s">
-        <v>163</v>
       </c>
       <c r="J45" s="97" t="s">
         <v>6</v>
       </c>
       <c r="K45" s="97" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L45" s="97" t="s">
         <v>27</v>
       </c>
       <c r="M45" s="64"/>
       <c r="N45" s="112" t="s">
+        <v>156</v>
+      </c>
+      <c r="O45" s="97" t="s">
+        <v>142</v>
+      </c>
+      <c r="P45" s="97" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q45" s="97" t="s">
         <v>158</v>
       </c>
-      <c r="O45" s="97" t="s">
-        <v>144</v>
-      </c>
-      <c r="P45" s="97" t="s">
+      <c r="R45" s="97" t="s">
         <v>159</v>
       </c>
-      <c r="Q45" s="97" t="s">
+      <c r="S45" s="97" t="s">
         <v>160</v>
       </c>
-      <c r="R45" s="97" t="s">
+      <c r="T45" s="97" t="s">
         <v>161</v>
-      </c>
-      <c r="S45" s="97" t="s">
-        <v>162</v>
-      </c>
-      <c r="T45" s="97" t="s">
-        <v>163</v>
       </c>
       <c r="U45" s="97" t="s">
         <v>6</v>
       </c>
       <c r="V45" s="97" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="W45" s="97" t="s">
         <v>27</v>
       </c>
       <c r="AB45" s="84" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AC45" s="84" t="s">
         <v>2</v>
       </c>
       <c r="AD45" s="84" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AE45" s="104" t="s">
         <v>3</v>
       </c>
       <c r="AF45" s="84" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AG45" s="84" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A46" s="138"/>
       <c r="B46" s="139"/>
       <c r="C46" s="69" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D46" s="100" t="e">
         <f>VLOOKUP($C46,SurveyData!$DQ:$DY,D$44,FALSE)</f>
@@ -10872,7 +10874,7 @@
       </c>
       <c r="M46" s="64"/>
       <c r="N46" s="69" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O46" s="72">
         <f>IFERROR(D46/$L$54,0)</f>
@@ -10911,7 +10913,7 @@
         <v>0</v>
       </c>
       <c r="AB46" s="84" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC46" s="82" t="e">
         <f>VLOOKUP(AB46,ModelData!EO:EP,2,FALSE)</f>
@@ -10934,11 +10936,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A47" s="138"/>
       <c r="B47" s="139"/>
       <c r="C47" s="69" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D47" s="100" t="e">
         <f>VLOOKUP($C47,SurveyData!$DQ:$DY,D$44,FALSE)</f>
@@ -10978,7 +10980,7 @@
       </c>
       <c r="M47" s="64"/>
       <c r="N47" s="69" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O47" s="72">
         <f t="shared" ref="O47:O54" si="37">IFERROR(D47/$L$54,0)</f>
@@ -11017,7 +11019,7 @@
         <v>0</v>
       </c>
       <c r="AB47" s="84" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC47" s="82" t="e">
         <f>VLOOKUP(AB47,ModelData!EO:EP,2,FALSE)</f>
@@ -11040,11 +11042,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A48" s="138"/>
       <c r="B48" s="139"/>
       <c r="C48" s="69" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D48" s="100" t="e">
         <f>VLOOKUP($C48,SurveyData!$DQ:$DY,D$44,FALSE)</f>
@@ -11084,7 +11086,7 @@
       </c>
       <c r="M48" s="64"/>
       <c r="N48" s="69" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O48" s="72">
         <f t="shared" si="37"/>
@@ -11123,7 +11125,7 @@
         <v>0</v>
       </c>
       <c r="AB48" s="84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AC48" s="82" t="e">
         <f>VLOOKUP(AB48,ModelData!EO:EP,2,FALSE)</f>
@@ -11146,11 +11148,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A49" s="138"/>
       <c r="B49" s="139"/>
       <c r="C49" s="69" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D49" s="100" t="e">
         <f>VLOOKUP($C49,SurveyData!$DQ:$DY,D$44,FALSE)</f>
@@ -11190,7 +11192,7 @@
       </c>
       <c r="M49" s="64"/>
       <c r="N49" s="69" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O49" s="72">
         <f t="shared" si="37"/>
@@ -11229,7 +11231,7 @@
         <v>0</v>
       </c>
       <c r="AB49" s="84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AC49" s="82" t="e">
         <f>VLOOKUP(AB49,ModelData!EO:EP,2,FALSE)</f>
@@ -11252,11 +11254,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A50" s="138"/>
       <c r="B50" s="139"/>
       <c r="C50" s="69" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D50" s="100" t="e">
         <f>VLOOKUP($C50,SurveyData!$DQ:$DY,D$44,FALSE)</f>
@@ -11296,7 +11298,7 @@
       </c>
       <c r="M50" s="64"/>
       <c r="N50" s="69" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O50" s="72">
         <f t="shared" si="37"/>
@@ -11335,7 +11337,7 @@
         <v>0</v>
       </c>
       <c r="AB50" s="84" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AC50" s="82" t="e">
         <f>VLOOKUP(AB50,ModelData!EO:EP,2,FALSE)</f>
@@ -11358,11 +11360,11 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A51" s="138"/>
       <c r="B51" s="139"/>
       <c r="C51" s="69" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D51" s="100" t="e">
         <f>VLOOKUP($C51,SurveyData!$DQ:$DY,D$44,FALSE)</f>
@@ -11402,7 +11404,7 @@
       </c>
       <c r="M51" s="64"/>
       <c r="N51" s="69" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O51" s="72">
         <f t="shared" si="37"/>
@@ -11455,7 +11457,7 @@
       <c r="AF51" s="89"/>
       <c r="AG51" s="84"/>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A52" s="138"/>
       <c r="B52" s="139"/>
       <c r="C52" s="69" t="s">
@@ -11538,11 +11540,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A53" s="138"/>
       <c r="B53" s="139"/>
       <c r="C53" s="69" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D53" s="100" t="e">
         <f>VLOOKUP($C53,SurveyData!$DQ:$DY,D$44,FALSE)</f>
@@ -11582,7 +11584,7 @@
       </c>
       <c r="M53" s="64"/>
       <c r="N53" s="69" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O53" s="72">
         <f t="shared" si="37"/>
@@ -11621,7 +11623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A54" s="138"/>
       <c r="B54" s="64"/>
       <c r="C54" s="71" t="s">
@@ -11704,7 +11706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A55" s="138"/>
       <c r="B55" s="64"/>
       <c r="C55" s="68"/>
@@ -11729,7 +11731,7 @@
       <c r="V55" s="64"/>
       <c r="W55" s="64"/>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A56" s="138"/>
       <c r="B56" s="64"/>
       <c r="C56" s="68"/>
@@ -11754,68 +11756,68 @@
       <c r="V56" s="64"/>
       <c r="W56" s="64"/>
     </row>
-    <row r="57" spans="1:37" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:37" ht="58" x14ac:dyDescent="0.35">
       <c r="A57" s="138"/>
       <c r="B57" s="139" t="s">
         <v>2</v>
       </c>
       <c r="C57" s="112" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D57" s="97" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E57" s="97" t="s">
+        <v>168</v>
+      </c>
+      <c r="F57" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="G57" s="97" t="s">
         <v>170</v>
       </c>
-      <c r="F57" s="97" t="s">
+      <c r="H57" s="97" t="s">
         <v>171</v>
       </c>
-      <c r="G57" s="97" t="s">
+      <c r="I57" s="97" t="s">
         <v>172</v>
       </c>
-      <c r="H57" s="97" t="s">
+      <c r="J57" s="97" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="97" t="s">
+      <c r="K57" s="97" t="s">
         <v>174</v>
-      </c>
-      <c r="J57" s="97" t="s">
-        <v>175</v>
-      </c>
-      <c r="K57" s="97" t="s">
-        <v>176</v>
       </c>
       <c r="L57" s="97" t="s">
         <v>27</v>
       </c>
       <c r="M57" s="64"/>
       <c r="N57" s="112" t="s">
+        <v>156</v>
+      </c>
+      <c r="O57" s="97" t="s">
+        <v>142</v>
+      </c>
+      <c r="P57" s="97" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q57" s="97" t="s">
         <v>158</v>
       </c>
-      <c r="O57" s="97" t="s">
-        <v>144</v>
-      </c>
-      <c r="P57" s="97" t="s">
+      <c r="R57" s="97" t="s">
         <v>159</v>
       </c>
-      <c r="Q57" s="97" t="s">
+      <c r="S57" s="97" t="s">
         <v>160</v>
       </c>
-      <c r="R57" s="97" t="s">
+      <c r="T57" s="97" t="s">
         <v>161</v>
-      </c>
-      <c r="S57" s="97" t="s">
-        <v>162</v>
-      </c>
-      <c r="T57" s="97" t="s">
-        <v>163</v>
       </c>
       <c r="U57" s="97" t="s">
         <v>6</v>
       </c>
       <c r="V57" s="97" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="W57" s="97" t="s">
         <v>27</v>
@@ -11824,11 +11826,11 @@
       <c r="AC57" s="64"/>
       <c r="AK57" s="64"/>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A58" s="138"/>
       <c r="B58" s="139"/>
       <c r="C58" s="69" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D58" s="99" t="e">
         <f>VLOOKUP($C58,ModelData!$DQ:$DY,D$44,FALSE)</f>
@@ -11868,7 +11870,7 @@
       </c>
       <c r="M58" s="64"/>
       <c r="N58" s="69" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O58" s="72">
         <f>IFERROR(D58/$L$66,0)</f>
@@ -11910,11 +11912,11 @@
       <c r="AC58" s="64"/>
       <c r="AK58" s="64"/>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A59" s="138"/>
       <c r="B59" s="139"/>
       <c r="C59" s="69" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D59" s="99" t="e">
         <f>VLOOKUP($C59,ModelData!$DQ:$DY,D$44,FALSE)</f>
@@ -11954,7 +11956,7 @@
       </c>
       <c r="M59" s="64"/>
       <c r="N59" s="69" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O59" s="72">
         <f t="shared" ref="O59:O66" si="45">IFERROR(D59/$L$66,0)</f>
@@ -11996,11 +11998,11 @@
       <c r="AC59" s="64"/>
       <c r="AK59" s="64"/>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A60" s="138"/>
       <c r="B60" s="139"/>
       <c r="C60" s="69" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D60" s="99" t="e">
         <f>VLOOKUP($C60,ModelData!$DQ:$DY,D$44,FALSE)</f>
@@ -12040,7 +12042,7 @@
       </c>
       <c r="M60" s="64"/>
       <c r="N60" s="69" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O60" s="72">
         <f t="shared" si="45"/>
@@ -12082,11 +12084,11 @@
       <c r="AC60" s="64"/>
       <c r="AK60" s="64"/>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A61" s="138"/>
       <c r="B61" s="139"/>
       <c r="C61" s="69" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D61" s="99" t="e">
         <f>VLOOKUP($C61,ModelData!$DQ:$DY,D$44,FALSE)</f>
@@ -12126,7 +12128,7 @@
       </c>
       <c r="M61" s="64"/>
       <c r="N61" s="69" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O61" s="72">
         <f t="shared" si="45"/>
@@ -12168,11 +12170,11 @@
       <c r="AC61" s="64"/>
       <c r="AK61" s="64"/>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A62" s="138"/>
       <c r="B62" s="139"/>
       <c r="C62" s="69" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D62" s="99" t="e">
         <f>VLOOKUP($C62,ModelData!$DQ:$DY,D$44,FALSE)</f>
@@ -12212,7 +12214,7 @@
       </c>
       <c r="M62" s="64"/>
       <c r="N62" s="69" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O62" s="72">
         <f t="shared" si="45"/>
@@ -12254,11 +12256,11 @@
       <c r="AC62" s="64"/>
       <c r="AK62" s="64"/>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A63" s="138"/>
       <c r="B63" s="139"/>
       <c r="C63" s="69" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D63" s="99" t="e">
         <f>VLOOKUP($C63,ModelData!$DQ:$DY,D$44,FALSE)</f>
@@ -12298,7 +12300,7 @@
       </c>
       <c r="M63" s="64"/>
       <c r="N63" s="69" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O63" s="72">
         <f t="shared" si="45"/>
@@ -12338,11 +12340,11 @@
       </c>
       <c r="AK63" s="64"/>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A64" s="138"/>
       <c r="B64" s="139"/>
       <c r="C64" s="69" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D64" s="99" t="e">
         <f>VLOOKUP($C64,ModelData!$DQ:$DY,D$44,FALSE)</f>
@@ -12421,11 +12423,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A65" s="138"/>
       <c r="B65" s="139"/>
       <c r="C65" s="69" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D65" s="99" t="e">
         <f>VLOOKUP($C65,ModelData!$DQ:$DY,D$44,FALSE)</f>
@@ -12465,7 +12467,7 @@
       </c>
       <c r="M65" s="64"/>
       <c r="N65" s="69" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O65" s="72">
         <f t="shared" si="45"/>
@@ -12504,7 +12506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A66" s="138"/>
       <c r="B66" s="64"/>
       <c r="C66" s="71" t="s">
@@ -12587,7 +12589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A67" s="138"/>
       <c r="B67" s="64"/>
       <c r="C67" s="68"/>
@@ -12612,7 +12614,7 @@
       <c r="V67" s="64"/>
       <c r="W67" s="64"/>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A68" s="138"/>
       <c r="B68" s="64"/>
       <c r="C68" s="68"/>
@@ -12637,7 +12639,7 @@
       <c r="V68" s="64"/>
       <c r="W68" s="64"/>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A69" s="138"/>
       <c r="B69" s="64"/>
       <c r="C69" s="68"/>
@@ -12662,7 +12664,7 @@
       <c r="V69" s="64"/>
       <c r="W69" s="64"/>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A70" s="138"/>
       <c r="B70" s="64"/>
       <c r="C70" s="68"/>
@@ -12687,7 +12689,7 @@
       <c r="V70" s="64"/>
       <c r="W70" s="64"/>
     </row>
-    <row r="71" spans="1:23" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:23" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="138"/>
       <c r="B71" s="64"/>
       <c r="C71" s="64"/>
@@ -12702,37 +12704,37 @@
       <c r="L71" s="64"/>
       <c r="M71" s="64"/>
       <c r="N71" s="112" t="s">
+        <v>156</v>
+      </c>
+      <c r="O71" s="101" t="s">
+        <v>142</v>
+      </c>
+      <c r="P71" s="101" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q71" s="101" t="s">
         <v>158</v>
       </c>
-      <c r="O71" s="101" t="s">
-        <v>144</v>
-      </c>
-      <c r="P71" s="101" t="s">
+      <c r="R71" s="101" t="s">
         <v>159</v>
       </c>
-      <c r="Q71" s="101" t="s">
+      <c r="S71" s="101" t="s">
         <v>160</v>
       </c>
-      <c r="R71" s="101" t="s">
+      <c r="T71" s="101" t="s">
         <v>161</v>
-      </c>
-      <c r="S71" s="101" t="s">
-        <v>162</v>
-      </c>
-      <c r="T71" s="101" t="s">
-        <v>163</v>
       </c>
       <c r="U71" s="101" t="s">
         <v>6</v>
       </c>
       <c r="V71" s="101" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="W71" s="101" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A72" s="138"/>
       <c r="B72" s="64"/>
       <c r="C72" s="64"/>
@@ -12747,7 +12749,7 @@
       <c r="L72" s="64"/>
       <c r="M72" s="64"/>
       <c r="N72" s="77" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O72" s="80">
         <f>O58-O46</f>
@@ -12786,7 +12788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A73" s="138"/>
       <c r="B73" s="64"/>
       <c r="C73" s="64"/>
@@ -12801,7 +12803,7 @@
       <c r="L73" s="64"/>
       <c r="M73" s="64"/>
       <c r="N73" s="77" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O73" s="80">
         <f t="shared" ref="O73:W80" si="48">O59-O47</f>
@@ -12840,7 +12842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A74" s="138"/>
       <c r="B74" s="64"/>
       <c r="C74" s="126"/>
@@ -12855,7 +12857,7 @@
       <c r="L74" s="64"/>
       <c r="M74" s="64"/>
       <c r="N74" s="77" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O74" s="80">
         <f t="shared" si="48"/>
@@ -12894,7 +12896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A75" s="138"/>
       <c r="B75" s="64"/>
       <c r="C75" s="126"/>
@@ -12909,7 +12911,7 @@
       <c r="L75" s="64"/>
       <c r="M75" s="64"/>
       <c r="N75" s="77" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O75" s="80">
         <f t="shared" si="48"/>
@@ -12948,7 +12950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A76" s="138"/>
       <c r="B76" s="64"/>
       <c r="C76" s="126"/>
@@ -12963,7 +12965,7 @@
       <c r="L76" s="64"/>
       <c r="M76" s="64"/>
       <c r="N76" s="77" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O76" s="80">
         <f t="shared" si="48"/>
@@ -13002,7 +13004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A77" s="138"/>
       <c r="B77" s="64"/>
       <c r="C77" s="126"/>
@@ -13017,7 +13019,7 @@
       <c r="L77" s="64"/>
       <c r="M77" s="64"/>
       <c r="N77" s="77" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O77" s="80">
         <f t="shared" si="48"/>
@@ -13056,7 +13058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A78" s="138"/>
       <c r="B78" s="64"/>
       <c r="C78" s="126"/>
@@ -13110,7 +13112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A79" s="138"/>
       <c r="B79" s="64"/>
       <c r="C79" s="126"/>
@@ -13125,7 +13127,7 @@
       <c r="L79" s="64"/>
       <c r="M79" s="64"/>
       <c r="N79" s="77" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O79" s="80">
         <f t="shared" si="48"/>
@@ -13164,7 +13166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A80" s="138"/>
       <c r="B80" s="64"/>
       <c r="C80" s="126"/>
@@ -13218,10 +13220,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="138"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="138"/>
     </row>
   </sheetData>
@@ -13296,17 +13298,17 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="15.76171875" customWidth="1"/>
-    <col min="6" max="6" width="20.234375" customWidth="1"/>
-    <col min="7" max="7" width="9.3515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.41015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:14" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="5:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E4" s="92" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F4" s="64"/>
       <c r="G4" s="64"/>
@@ -13315,7 +13317,7 @@
       <c r="J4" s="64"/>
       <c r="K4" s="64"/>
     </row>
-    <row r="5" spans="5:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E5" s="64"/>
       <c r="F5" s="64"/>
       <c r="G5" s="64"/>
@@ -13324,35 +13326,35 @@
       <c r="J5" s="64"/>
       <c r="K5" s="64"/>
     </row>
-    <row r="6" spans="5:14" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="5:14" ht="29" x14ac:dyDescent="0.35">
       <c r="E6" s="67" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="G6" s="66" t="s">
         <v>180</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="H6" s="66" t="s">
         <v>181</v>
       </c>
-      <c r="G6" s="66" t="s">
+      <c r="I6" s="66" t="s">
         <v>182</v>
       </c>
-      <c r="H6" s="66" t="s">
+      <c r="J6" s="66" t="s">
         <v>183</v>
       </c>
-      <c r="I6" s="66" t="s">
+      <c r="K6" s="66" t="s">
         <v>184</v>
       </c>
-      <c r="J6" s="66" t="s">
-        <v>185</v>
-      </c>
-      <c r="K6" s="66" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="5:14" x14ac:dyDescent="0.5">
+    </row>
+    <row r="7" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E7" s="71" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F7" s="90" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G7" s="70" t="e">
         <f>VLOOKUP(F7,ModelData!DH:DI,2,FALSE)</f>
@@ -13375,15 +13377,15 @@
         <v>#N/A</v>
       </c>
       <c r="N7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="5:14" x14ac:dyDescent="0.5">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E8" s="71" t="s">
         <v>115</v>
       </c>
       <c r="F8" s="90" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G8" s="70" t="e">
         <f>VLOOKUP(F8,ModelData!DH:DI,2,FALSE)</f>
@@ -13409,12 +13411,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="5:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E9" s="71" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F9" s="90" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G9" s="70" t="e">
         <f>VLOOKUP(F9,ModelData!DH:DI,2,FALSE)</f>
@@ -13437,15 +13439,15 @@
         <v>#N/A</v>
       </c>
       <c r="N9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E10" s="71" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="10" spans="5:14" x14ac:dyDescent="0.5">
-      <c r="E10" s="71" t="s">
-        <v>146</v>
-      </c>
       <c r="F10" s="90" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G10" s="70" t="e">
         <f>VLOOKUP(F10,ModelData!DH:DI,2,FALSE)</f>
@@ -13468,15 +13470,15 @@
         <v>#N/A</v>
       </c>
       <c r="N10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="5:14" x14ac:dyDescent="0.5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E11" s="71" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F11" s="90" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G11" s="70" t="e">
         <f>VLOOKUP(F11,ModelData!DH:DI,2,FALSE)</f>
@@ -13499,45 +13501,45 @@
         <v>#N/A</v>
       </c>
       <c r="N11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="5:14" x14ac:dyDescent="0.5">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E12" s="71" t="s">
         <v>27</v>
       </c>
       <c r="F12" s="90" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G12" s="91" t="e">
         <f>SUM(G7:G11)</f>
         <v>#N/A</v>
       </c>
       <c r="H12" s="90" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I12" s="91" t="e">
         <f>SUM(I7:I11)</f>
         <v>#N/A</v>
       </c>
       <c r="J12" s="90" t="s">
+        <v>187</v>
+      </c>
+      <c r="K12" s="90" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="F17" s="94" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="142" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="95" t="s">
         <v>189</v>
-      </c>
-      <c r="K12" s="90" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.6">
-      <c r="F17" s="94" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A19" s="142" t="s">
-        <v>154</v>
-      </c>
-      <c r="F19" s="95" t="s">
-        <v>191</v>
       </c>
       <c r="G19" s="96" t="s">
         <v>2</v>
@@ -13549,7 +13551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="142"/>
       <c r="F20" s="71" t="s">
         <v>119</v>
@@ -13567,7 +13569,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="142"/>
       <c r="F21" s="71" t="s">
         <v>121</v>
@@ -13585,7 +13587,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F22" s="71" t="s">
         <v>120</v>
       </c>
@@ -13602,17 +13604,17 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="F25" s="94" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="143" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F27" s="95" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G27" s="96" t="s">
         <v>2</v>
@@ -13624,7 +13626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="143"/>
       <c r="F28" s="71" t="s">
         <v>119</v>
@@ -13642,7 +13644,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="143"/>
       <c r="F29" s="71" t="s">
         <v>121</v>
@@ -13651,7 +13653,7 @@
       <c r="H29" s="124"/>
       <c r="I29" s="72"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F30" s="71" t="s">
         <v>120</v>
       </c>
@@ -13714,19 +13716,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="608512b1-9b7f-4b66-9287-846c132e154a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="8a8ccdf0-e2fe-48b3-ba2f-122b2fdfcc3b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5D9AA5C7921F342991554F4D6B3A08A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0206a618f35c0824d2fb24aead71b636">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="608512b1-9b7f-4b66-9287-846c132e154a" xmlns:ns3="8a8ccdf0-e2fe-48b3-ba2f-122b2fdfcc3b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="92f8997cce93524906d692cae9c8e282" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -13966,6 +13955,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="608512b1-9b7f-4b66-9287-846c132e154a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="8a8ccdf0-e2fe-48b3-ba2f-122b2fdfcc3b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86BB1708-1A79-483C-A626-7FB01DBF8F72}">
   <ds:schemaRefs>
@@ -13975,24 +13977,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2752ED4C-9964-4342-8BFC-8B13FAE1D1E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="608512b1-9b7f-4b66-9287-846c132e154a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="8a8ccdf0-e2fe-48b3-ba2f-122b2fdfcc3b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D2D9C9-6CE7-42B3-B73E-F50E2DED2FCF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14010,4 +13994,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2752ED4C-9964-4342-8BFC-8B13FAE1D1E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="608512b1-9b7f-4b66-9287-846c132e154a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="8a8ccdf0-e2fe-48b3-ba2f-122b2fdfcc3b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>